<commit_message>
Added a new report forlder. Also added the files needed to run the C16h16_chair structure.
</commit_message>
<xml_diff>
--- a/100h_c16h16_chair_MT/conversion_angstroms-bohrs.xlsx
+++ b/100h_c16h16_chair_MT/conversion_angstroms-bohrs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>angstrom=</t>
   </si>
@@ -27,18 +27,42 @@
   </si>
   <si>
     <t>angstroms</t>
+  </si>
+  <si>
+    <t>Angstroms</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Bohrs</t>
+  </si>
+  <si>
+    <t>Distance x</t>
+  </si>
+  <si>
+    <t>Angstroms:</t>
+  </si>
+  <si>
+    <t>Distance y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="0" numFmtId="165"/>
+    <numFmt formatCode="0.000000000" numFmtId="166"/>
   </numFmts>
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -100,8 +124,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -119,43 +148,410 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100">
-      <selection activeCell="I1" activeCellId="0" pane="topLeft" sqref="I1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100">
+      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.74117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.3019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.6509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="2.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="6.07058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="11.6509803921569"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="9.92941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <v>1.889725989</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="0" t="n">
+      <c r="F1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="0" t="n">
+      <c r="H1" s="2" t="n">
         <v>0.529177249</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="2">
+      <c r="C2" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="3">
+      <c r="C3" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="4">
+      <c r="C4" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="5">
+      <c r="C5" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="6">
+      <c r="C6" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="7">
+      <c r="C7" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="8">
+      <c r="C8" s="2" t="n">
+        <v>1.889725989</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>-2.38E-007</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>-5.41E-006</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>13.612187386</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>-2.38E-007</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1.420668721</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10.925222397</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>1.230336905</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2.131008625</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>13.61218071</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1.230336905</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>3.551680088</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>10.925221443</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>-2.38E-007</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>2.29E-007</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>12.49555397</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>-2.38E-007</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1.420670629</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>12.04189682</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>1.230336905</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2.131008148</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>12.495545387</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>1.230336905</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>3.551676035</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>12.041895866</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="1" t="str">
+        <f aca="false">A10</f>
+        <v>H</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <f aca="false">B10*C1</f>
+        <v>-4.49754785382E-007</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <f aca="false">C10*C1</f>
+        <v>-1.022341760049E-005</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <f aca="false">D10*C1</f>
+        <v>25.7233042704622</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="1" t="str">
+        <f aca="false">A11</f>
+        <v>H</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <f aca="false">B11*C2</f>
+        <v>-4.49754785382E-007</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <f aca="false">C11*C2</f>
+        <v>2.68467460383309</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <f aca="false">D11*C2</f>
+        <v>20.6456766992158</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="1" t="str">
+        <f aca="false">A12</f>
+        <v>H</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <f aca="false">B12*C3</f>
+        <v>2.32499962460432</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <f aca="false">C12*C3</f>
+        <v>4.02702238144566</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <f aca="false">D12*C3</f>
+        <v>25.7232916546515</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="1" t="str">
+        <f aca="false">A13</f>
+        <v>H</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <f aca="false">B13*C4</f>
+        <v>2.32499962460432</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <f aca="false">C13*C4</f>
+        <v>6.71170216690741</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <f aca="false">D13*C4</f>
+        <v>20.6456748964172</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="1" t="str">
+        <f aca="false">A14</f>
+        <v>C</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <f aca="false">B14*C5</f>
+        <v>-4.49754785382E-007</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <f aca="false">C14*C5</f>
+        <v>4.32747251481E-007</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <f aca="false">D14*C5</f>
+        <v>23.6131730840611</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="1" t="str">
+        <f aca="false">A15</f>
+        <v>C</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <f aca="false">B15*C6</f>
+        <v>-4.49754785382E-007</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <f aca="false">C15*C6</f>
+        <v>2.68467820943028</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <f aca="false">D15*C6</f>
+        <v>22.7558853776105</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="1" t="str">
+        <f aca="false">A16</f>
+        <v>C</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <f aca="false">B16*C7</f>
+        <v>2.32499962460432</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <f aca="false">C16*C7</f>
+        <v>4.02702148004636</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <f aca="false">D16*C7</f>
+        <v>23.613156864543</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="1" t="str">
+        <f aca="false">A17</f>
+        <v>C</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <f aca="false">B17*C8</f>
+        <v>2.32499962460432</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <f aca="false">C17*C8</f>
+        <v>6.71169450784797</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <f aca="false">D17*C8</f>
+        <v>22.7558835748119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <f aca="false">(2.460673809+0.000000238)</f>
+        <v>2.460674047</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="B31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <f aca="false">C30*C1</f>
+        <v>4.64999969707371</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="B33" s="0"/>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <f aca="false">(4.262012482-0.000000229)</f>
+        <v>4.262012253</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="B35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <f aca="false">C34*C1</f>
+        <v>8.05403531993054</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A19:D19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>

<commit_message>
Checking mistakes because the structure seems to be a metal.
</commit_message>
<xml_diff>
--- a/100h_c16h16_chair_MT/conversion_angstroms-bohrs.xlsx
+++ b/100h_c16h16_chair_MT/conversion_angstroms-bohrs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>angstrom=</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>Bohrs</t>
+  </si>
+  <si>
+    <t>posx1</t>
+  </si>
+  <si>
+    <t>posx2</t>
+  </si>
+  <si>
+    <t>Distx</t>
+  </si>
+  <si>
+    <t>Posy1</t>
+  </si>
+  <si>
+    <t>Posy2</t>
   </si>
   <si>
     <t>Distance x</t>
@@ -128,7 +143,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
   </cellXfs>
@@ -151,20 +166,20 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100">
-      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
+      <selection activeCell="J27" activeCellId="0" pane="topLeft" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.74117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.3019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.6509803921569"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="2.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="6.07058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="11.6509803921569"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="9.92941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.74901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.3647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.7137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.678431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="2.42352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="6.10588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="11.7137254901961"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="1">
@@ -228,7 +243,7 @@
         <v>1.889725989</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -236,7 +251,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -250,7 +265,7 @@
         <v>13.612187386</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -264,7 +279,7 @@
         <v>10.925222397</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -278,7 +293,7 @@
         <v>13.61218071</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -292,7 +307,7 @@
         <v>10.925221443</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -306,7 +321,7 @@
         <v>12.49555397</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -320,7 +335,7 @@
         <v>12.04189682</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -334,7 +349,7 @@
         <v>12.495545387</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -348,7 +363,7 @@
         <v>12.041895866</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -356,7 +371,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="1" t="str">
         <f aca="false">A10</f>
         <v>H</v>
@@ -374,7 +389,7 @@
         <v>25.7233042704622</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="1" t="str">
         <f aca="false">A11</f>
         <v>H</v>
@@ -392,7 +407,7 @@
         <v>20.6456766992158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="1" t="str">
         <f aca="false">A12</f>
         <v>H</v>
@@ -409,8 +424,14 @@
         <f aca="false">D12*C3</f>
         <v>25.7232916546515</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="H22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="1" t="str">
         <f aca="false">A13</f>
         <v>H</v>
@@ -427,8 +448,14 @@
         <f aca="false">D13*C4</f>
         <v>20.6456748964172</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="H23" s="2" t="n">
+        <v>2.460673809</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>-2.38E-007</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="1" t="str">
         <f aca="false">A14</f>
         <v>C</v>
@@ -446,7 +473,7 @@
         <v>23.6131730840611</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="1" t="str">
         <f aca="false">A15</f>
         <v>C</v>
@@ -463,8 +490,11 @@
         <f aca="false">D15*C6</f>
         <v>22.7558853776105</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="H25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="1" t="str">
         <f aca="false">A16</f>
         <v>C</v>
@@ -481,8 +511,12 @@
         <f aca="false">D16*C7</f>
         <v>23.613156864543</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="H26" s="2" t="n">
+        <f aca="false">H23-I23</f>
+        <v>2.460674047</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="1" t="str">
         <f aca="false">A17</f>
         <v>C</v>
@@ -500,21 +534,39 @@
         <v>22.7558835748119</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="H28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="C29" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+        <v>13</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>2.29E-007</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>4.262012482</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="B30" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C30" s="2" t="n">
         <f aca="false">(2.460673809+0.000000238)</f>
         <v>2.460674047</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="H30" s="2" t="n">
+        <f aca="false">I29-H29</f>
+        <v>4.262012253</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
@@ -523,22 +575,21 @@
         <v>4.64999969707371</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="B33" s="0"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="C33" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C34" s="2" t="n">
         <f aca="false">(4.262012482-0.000000229)</f>
         <v>4.262012253</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>